<commit_message>
added gpt + some fixes
</commit_message>
<xml_diff>
--- a/boosting_input_all_categories.xlsx
+++ b/boosting_input_all_categories.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,184 +456,106 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45776</v>
+        <v>45779</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Аптеки</t>
+          <t>Бытовые услуги</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3209</v>
+        <v>432</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45776</v>
+        <v>45779</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Бытовые услуги</t>
+          <t>Кафе, рестораны, фастфуд</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>432</v>
+        <v>28857</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45776</v>
+        <v>45779</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ЖКХ; связь; интернет</t>
+          <t>Комиссия</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45776</v>
+        <v>45779</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Кафе, рестораны, фастфуд</t>
+          <t>Одежда и обувь</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>44263</v>
+        <v>16469</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45776</v>
+        <v>45779</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Комиссия</t>
+          <t>Путешествия</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>200</v>
+        <v>117704</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45776</v>
+        <v>45779</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Медицинские услуги</t>
+          <t>Супермаркеты</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>25503</v>
+        <v>7989</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45776</v>
+        <v>45779</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Одежда и</t>
+          <t>Такси и каршеринг</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7505</v>
+        <v>6584</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45776</v>
+        <v>45779</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Одежда и обувь</t>
+          <t>Хобби и развлечения</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16469</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>45776</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Перевозка, доставка</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>45776</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Путешествия</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>117704</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>45776</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Супермаркеты</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>26028</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>45776</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Такси и каршеринг</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>19990</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
-        <v>45776</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Транспорт</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>45776</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Хобби и развлечения</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>15220</v>
+        <v>7870</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
devide buttons and analytics
</commit_message>
<xml_diff>
--- a/boosting_input_all_categories.xlsx
+++ b/boosting_input_all_categories.xlsx
@@ -456,7 +456,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45779</v>
+        <v>45780</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -469,7 +469,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45779</v>
+        <v>45780</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -482,7 +482,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45779</v>
+        <v>45780</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -495,7 +495,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45779</v>
+        <v>45780</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -508,7 +508,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45779</v>
+        <v>45780</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -521,7 +521,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45779</v>
+        <v>45780</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -534,7 +534,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45779</v>
+        <v>45780</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -547,7 +547,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45779</v>
+        <v>45780</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>

</xml_diff>